<commit_message>
add annotations by nils
</commit_message>
<xml_diff>
--- a/Datasets/annotated_dataset/tweets_session_1_1.xlsx
+++ b/Datasets/annotated_dataset/tweets_session_1_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils_hellwig/Desktop/Studium/Masterstudium WS 2022:23/DH Projekt/Twitter_German_Federal_Election_Perception_2021/Datasets/annotated_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EC935A-95D2-8F45-B9FD-872D2DA83CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4191AB88-FDAE-DC45-9C0F-26F8EDF2EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6708" uniqueCount="4057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7008" uniqueCount="4057">
   <si>
     <t>id</t>
   </si>
@@ -12556,8 +12556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B667" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="E702" sqref="E702"/>
+    <sheetView tabSelected="1" topLeftCell="A977" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <selection activeCell="E997" sqref="E997"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -32908,6 +32908,9 @@
       <c r="D702" t="s">
         <v>2866</v>
       </c>
+      <c r="E702" t="s">
+        <v>4054</v>
+      </c>
       <c r="F702" t="s">
         <v>2867</v>
       </c>
@@ -32934,6 +32937,9 @@
       <c r="D703" t="s">
         <v>2870</v>
       </c>
+      <c r="E703" t="s">
+        <v>4054</v>
+      </c>
       <c r="F703" t="s">
         <v>2871</v>
       </c>
@@ -32960,6 +32966,9 @@
       <c r="D704" t="s">
         <v>2874</v>
       </c>
+      <c r="E704" t="s">
+        <v>4055</v>
+      </c>
       <c r="F704" t="s">
         <v>2875</v>
       </c>
@@ -32986,6 +32995,9 @@
       <c r="D705" t="s">
         <v>2878</v>
       </c>
+      <c r="E705" t="s">
+        <v>4054</v>
+      </c>
       <c r="F705" t="s">
         <v>2879</v>
       </c>
@@ -33012,6 +33024,9 @@
       <c r="D706" t="s">
         <v>2882</v>
       </c>
+      <c r="E706" t="s">
+        <v>4054</v>
+      </c>
       <c r="F706" t="s">
         <v>2883</v>
       </c>
@@ -33038,6 +33053,9 @@
       <c r="D707" t="s">
         <v>2886</v>
       </c>
+      <c r="E707" t="s">
+        <v>4054</v>
+      </c>
       <c r="F707" t="s">
         <v>2887</v>
       </c>
@@ -33064,6 +33082,9 @@
       <c r="D708" t="s">
         <v>2890</v>
       </c>
+      <c r="E708" t="s">
+        <v>4056</v>
+      </c>
       <c r="F708" t="s">
         <v>2891</v>
       </c>
@@ -33090,6 +33111,9 @@
       <c r="D709" t="s">
         <v>2894</v>
       </c>
+      <c r="E709" t="s">
+        <v>4053</v>
+      </c>
       <c r="F709" t="s">
         <v>2895</v>
       </c>
@@ -33116,6 +33140,9 @@
       <c r="D710" t="s">
         <v>2898</v>
       </c>
+      <c r="E710" t="s">
+        <v>4055</v>
+      </c>
       <c r="F710" t="s">
         <v>2899</v>
       </c>
@@ -33142,6 +33169,9 @@
       <c r="D711" t="s">
         <v>2902</v>
       </c>
+      <c r="E711" t="s">
+        <v>4053</v>
+      </c>
       <c r="F711" t="s">
         <v>2903</v>
       </c>
@@ -33168,6 +33198,9 @@
       <c r="D712" t="s">
         <v>2906</v>
       </c>
+      <c r="E712" t="s">
+        <v>4055</v>
+      </c>
       <c r="F712" t="s">
         <v>2907</v>
       </c>
@@ -33194,6 +33227,9 @@
       <c r="D713" t="s">
         <v>2910</v>
       </c>
+      <c r="E713" t="s">
+        <v>4053</v>
+      </c>
       <c r="F713" t="s">
         <v>2911</v>
       </c>
@@ -33220,6 +33256,9 @@
       <c r="D714" t="s">
         <v>2914</v>
       </c>
+      <c r="E714" t="s">
+        <v>4053</v>
+      </c>
       <c r="F714" t="s">
         <v>2915</v>
       </c>
@@ -33246,6 +33285,9 @@
       <c r="D715" t="s">
         <v>2918</v>
       </c>
+      <c r="E715" t="s">
+        <v>4054</v>
+      </c>
       <c r="F715" t="s">
         <v>2919</v>
       </c>
@@ -33272,6 +33314,9 @@
       <c r="D716" t="s">
         <v>2922</v>
       </c>
+      <c r="E716" t="s">
+        <v>4054</v>
+      </c>
       <c r="F716" t="s">
         <v>2923</v>
       </c>
@@ -33298,6 +33343,9 @@
       <c r="D717" t="s">
         <v>2926</v>
       </c>
+      <c r="E717" t="s">
+        <v>4053</v>
+      </c>
       <c r="F717" t="s">
         <v>2927</v>
       </c>
@@ -33324,6 +33372,9 @@
       <c r="D718" t="s">
         <v>2929</v>
       </c>
+      <c r="E718" t="s">
+        <v>4054</v>
+      </c>
       <c r="F718" t="s">
         <v>2930</v>
       </c>
@@ -33350,6 +33401,9 @@
       <c r="D719" t="s">
         <v>2933</v>
       </c>
+      <c r="E719" t="s">
+        <v>4054</v>
+      </c>
       <c r="F719" t="s">
         <v>2934</v>
       </c>
@@ -33376,6 +33430,9 @@
       <c r="D720" t="s">
         <v>2937</v>
       </c>
+      <c r="E720" t="s">
+        <v>4054</v>
+      </c>
       <c r="F720" t="s">
         <v>2938</v>
       </c>
@@ -33402,6 +33459,9 @@
       <c r="D721" t="s">
         <v>2941</v>
       </c>
+      <c r="E721" t="s">
+        <v>4053</v>
+      </c>
       <c r="F721" t="s">
         <v>2942</v>
       </c>
@@ -33428,6 +33488,9 @@
       <c r="D722" t="s">
         <v>2945</v>
       </c>
+      <c r="E722" t="s">
+        <v>4053</v>
+      </c>
       <c r="F722" t="s">
         <v>2946</v>
       </c>
@@ -33454,6 +33517,9 @@
       <c r="D723" t="s">
         <v>2949</v>
       </c>
+      <c r="E723" t="s">
+        <v>4053</v>
+      </c>
       <c r="F723" t="s">
         <v>2950</v>
       </c>
@@ -33480,6 +33546,9 @@
       <c r="D724" t="s">
         <v>2953</v>
       </c>
+      <c r="E724" t="s">
+        <v>4054</v>
+      </c>
       <c r="F724" t="s">
         <v>2954</v>
       </c>
@@ -33506,6 +33575,9 @@
       <c r="D725" t="s">
         <v>2957</v>
       </c>
+      <c r="E725" t="s">
+        <v>4054</v>
+      </c>
       <c r="F725" t="s">
         <v>2958</v>
       </c>
@@ -33532,6 +33604,9 @@
       <c r="D726" t="s">
         <v>2961</v>
       </c>
+      <c r="E726" t="s">
+        <v>4054</v>
+      </c>
       <c r="F726" t="s">
         <v>2962</v>
       </c>
@@ -33558,6 +33633,9 @@
       <c r="D727" t="s">
         <v>2965</v>
       </c>
+      <c r="E727" t="s">
+        <v>4054</v>
+      </c>
       <c r="F727" t="s">
         <v>2966</v>
       </c>
@@ -33584,6 +33662,9 @@
       <c r="D728" t="s">
         <v>2969</v>
       </c>
+      <c r="E728" t="s">
+        <v>4053</v>
+      </c>
       <c r="F728" t="s">
         <v>2970</v>
       </c>
@@ -33610,6 +33691,9 @@
       <c r="D729" t="s">
         <v>2973</v>
       </c>
+      <c r="E729" t="s">
+        <v>4053</v>
+      </c>
       <c r="F729" t="s">
         <v>2974</v>
       </c>
@@ -33636,6 +33720,9 @@
       <c r="D730" t="s">
         <v>2977</v>
       </c>
+      <c r="E730" t="s">
+        <v>4053</v>
+      </c>
       <c r="F730" t="s">
         <v>2978</v>
       </c>
@@ -33662,6 +33749,9 @@
       <c r="D731" t="s">
         <v>2981</v>
       </c>
+      <c r="E731" t="s">
+        <v>4053</v>
+      </c>
       <c r="F731" t="s">
         <v>2982</v>
       </c>
@@ -33688,6 +33778,9 @@
       <c r="D732" t="s">
         <v>2985</v>
       </c>
+      <c r="E732" t="s">
+        <v>4054</v>
+      </c>
       <c r="F732" t="s">
         <v>2986</v>
       </c>
@@ -33714,6 +33807,9 @@
       <c r="D733" t="s">
         <v>2989</v>
       </c>
+      <c r="E733" t="s">
+        <v>4055</v>
+      </c>
       <c r="F733" t="s">
         <v>2990</v>
       </c>
@@ -33740,6 +33836,9 @@
       <c r="D734" t="s">
         <v>2993</v>
       </c>
+      <c r="E734" t="s">
+        <v>4053</v>
+      </c>
       <c r="F734" t="s">
         <v>2994</v>
       </c>
@@ -33766,6 +33865,9 @@
       <c r="D735" t="s">
         <v>2997</v>
       </c>
+      <c r="E735" t="s">
+        <v>4053</v>
+      </c>
       <c r="F735" t="s">
         <v>2998</v>
       </c>
@@ -33792,6 +33894,9 @@
       <c r="D736" t="s">
         <v>3001</v>
       </c>
+      <c r="E736" t="s">
+        <v>4053</v>
+      </c>
       <c r="F736" t="s">
         <v>3002</v>
       </c>
@@ -33818,6 +33923,9 @@
       <c r="D737" t="s">
         <v>3005</v>
       </c>
+      <c r="E737" t="s">
+        <v>4053</v>
+      </c>
       <c r="F737" t="s">
         <v>3006</v>
       </c>
@@ -33844,6 +33952,9 @@
       <c r="D738" t="s">
         <v>3009</v>
       </c>
+      <c r="E738" t="s">
+        <v>4054</v>
+      </c>
       <c r="F738" t="s">
         <v>3010</v>
       </c>
@@ -33870,6 +33981,9 @@
       <c r="D739" t="s">
         <v>3013</v>
       </c>
+      <c r="E739" t="s">
+        <v>4054</v>
+      </c>
       <c r="F739" t="s">
         <v>3014</v>
       </c>
@@ -33896,6 +34010,9 @@
       <c r="D740" t="s">
         <v>3017</v>
       </c>
+      <c r="E740" t="s">
+        <v>4054</v>
+      </c>
       <c r="F740" t="s">
         <v>3018</v>
       </c>
@@ -33922,6 +34039,9 @@
       <c r="D741" t="s">
         <v>3021</v>
       </c>
+      <c r="E741" t="s">
+        <v>4053</v>
+      </c>
       <c r="F741" t="s">
         <v>3022</v>
       </c>
@@ -33948,6 +34068,9 @@
       <c r="D742" t="s">
         <v>3025</v>
       </c>
+      <c r="E742" t="s">
+        <v>4054</v>
+      </c>
       <c r="F742" t="s">
         <v>3026</v>
       </c>
@@ -33974,6 +34097,9 @@
       <c r="D743" t="s">
         <v>3029</v>
       </c>
+      <c r="E743" t="s">
+        <v>4054</v>
+      </c>
       <c r="F743" t="s">
         <v>3030</v>
       </c>
@@ -34000,6 +34126,9 @@
       <c r="D744" t="s">
         <v>3033</v>
       </c>
+      <c r="E744" t="s">
+        <v>4054</v>
+      </c>
       <c r="F744" t="s">
         <v>3034</v>
       </c>
@@ -34026,6 +34155,9 @@
       <c r="D745" t="s">
         <v>3037</v>
       </c>
+      <c r="E745" t="s">
+        <v>4054</v>
+      </c>
       <c r="F745" t="s">
         <v>3038</v>
       </c>
@@ -34052,6 +34184,9 @@
       <c r="D746" t="s">
         <v>3041</v>
       </c>
+      <c r="E746" t="s">
+        <v>4054</v>
+      </c>
       <c r="F746" t="s">
         <v>3042</v>
       </c>
@@ -34078,6 +34213,9 @@
       <c r="D747" t="s">
         <v>3045</v>
       </c>
+      <c r="E747" t="s">
+        <v>4054</v>
+      </c>
       <c r="F747" t="s">
         <v>3046</v>
       </c>
@@ -34104,6 +34242,9 @@
       <c r="D748" t="s">
         <v>3049</v>
       </c>
+      <c r="E748" t="s">
+        <v>4053</v>
+      </c>
       <c r="F748" t="s">
         <v>3050</v>
       </c>
@@ -34130,6 +34271,9 @@
       <c r="D749" t="s">
         <v>3053</v>
       </c>
+      <c r="E749" t="s">
+        <v>4054</v>
+      </c>
       <c r="F749" t="s">
         <v>3054</v>
       </c>
@@ -34156,6 +34300,9 @@
       <c r="D750" t="s">
         <v>3057</v>
       </c>
+      <c r="E750" t="s">
+        <v>4054</v>
+      </c>
       <c r="F750" t="s">
         <v>3058</v>
       </c>
@@ -34182,6 +34329,9 @@
       <c r="D751" t="s">
         <v>3061</v>
       </c>
+      <c r="E751" t="s">
+        <v>4053</v>
+      </c>
       <c r="F751" t="s">
         <v>3062</v>
       </c>
@@ -34208,6 +34358,9 @@
       <c r="D752" t="s">
         <v>3065</v>
       </c>
+      <c r="E752" t="s">
+        <v>4054</v>
+      </c>
       <c r="F752" t="s">
         <v>3066</v>
       </c>
@@ -34234,6 +34387,9 @@
       <c r="D753" t="s">
         <v>3069</v>
       </c>
+      <c r="E753" t="s">
+        <v>4054</v>
+      </c>
       <c r="F753" t="s">
         <v>3070</v>
       </c>
@@ -34260,6 +34416,9 @@
       <c r="D754" t="s">
         <v>3073</v>
       </c>
+      <c r="E754" t="s">
+        <v>4053</v>
+      </c>
       <c r="F754" t="s">
         <v>3074</v>
       </c>
@@ -34286,6 +34445,9 @@
       <c r="D755" t="s">
         <v>3077</v>
       </c>
+      <c r="E755" t="s">
+        <v>4053</v>
+      </c>
       <c r="F755" t="s">
         <v>3078</v>
       </c>
@@ -34312,6 +34474,9 @@
       <c r="D756" t="s">
         <v>3081</v>
       </c>
+      <c r="E756" t="s">
+        <v>4053</v>
+      </c>
       <c r="F756" t="s">
         <v>3082</v>
       </c>
@@ -34338,6 +34503,9 @@
       <c r="D757" t="s">
         <v>3085</v>
       </c>
+      <c r="E757" t="s">
+        <v>4053</v>
+      </c>
       <c r="F757" t="s">
         <v>3086</v>
       </c>
@@ -34364,6 +34532,9 @@
       <c r="D758" t="s">
         <v>3089</v>
       </c>
+      <c r="E758" t="s">
+        <v>4056</v>
+      </c>
       <c r="F758" t="s">
         <v>3090</v>
       </c>
@@ -34390,6 +34561,9 @@
       <c r="D759" t="s">
         <v>3093</v>
       </c>
+      <c r="E759" t="s">
+        <v>4054</v>
+      </c>
       <c r="F759" t="s">
         <v>3094</v>
       </c>
@@ -34416,6 +34590,9 @@
       <c r="D760" t="s">
         <v>3097</v>
       </c>
+      <c r="E760" t="s">
+        <v>4053</v>
+      </c>
       <c r="F760" t="s">
         <v>3098</v>
       </c>
@@ -34442,6 +34619,9 @@
       <c r="D761" t="s">
         <v>3101</v>
       </c>
+      <c r="E761" t="s">
+        <v>4054</v>
+      </c>
       <c r="F761" t="s">
         <v>3102</v>
       </c>
@@ -34468,6 +34648,9 @@
       <c r="D762" t="s">
         <v>3105</v>
       </c>
+      <c r="E762" t="s">
+        <v>4053</v>
+      </c>
       <c r="F762" t="s">
         <v>3106</v>
       </c>
@@ -34494,6 +34677,9 @@
       <c r="D763" t="s">
         <v>3109</v>
       </c>
+      <c r="E763" t="s">
+        <v>4054</v>
+      </c>
       <c r="F763" t="s">
         <v>3110</v>
       </c>
@@ -34520,6 +34706,9 @@
       <c r="D764" t="s">
         <v>3113</v>
       </c>
+      <c r="E764" t="s">
+        <v>4054</v>
+      </c>
       <c r="F764" t="s">
         <v>3114</v>
       </c>
@@ -34546,6 +34735,9 @@
       <c r="D765" t="s">
         <v>3117</v>
       </c>
+      <c r="E765" t="s">
+        <v>4054</v>
+      </c>
       <c r="F765" t="s">
         <v>3118</v>
       </c>
@@ -34572,6 +34764,9 @@
       <c r="D766" t="s">
         <v>3121</v>
       </c>
+      <c r="E766" t="s">
+        <v>4053</v>
+      </c>
       <c r="F766" t="s">
         <v>3122</v>
       </c>
@@ -34598,6 +34793,9 @@
       <c r="D767" t="s">
         <v>3125</v>
       </c>
+      <c r="E767" t="s">
+        <v>4054</v>
+      </c>
       <c r="F767" t="s">
         <v>3126</v>
       </c>
@@ -34624,6 +34822,9 @@
       <c r="D768" t="s">
         <v>3129</v>
       </c>
+      <c r="E768" t="s">
+        <v>4055</v>
+      </c>
       <c r="F768" t="s">
         <v>3130</v>
       </c>
@@ -34650,6 +34851,9 @@
       <c r="D769" t="s">
         <v>3133</v>
       </c>
+      <c r="E769" t="s">
+        <v>4054</v>
+      </c>
       <c r="F769" t="s">
         <v>3134</v>
       </c>
@@ -34676,6 +34880,9 @@
       <c r="D770" t="s">
         <v>3137</v>
       </c>
+      <c r="E770" t="s">
+        <v>4054</v>
+      </c>
       <c r="F770" t="s">
         <v>3138</v>
       </c>
@@ -34702,6 +34909,9 @@
       <c r="D771" t="s">
         <v>3141</v>
       </c>
+      <c r="E771" t="s">
+        <v>4054</v>
+      </c>
       <c r="F771" t="s">
         <v>3142</v>
       </c>
@@ -34728,6 +34938,9 @@
       <c r="D772" t="s">
         <v>3145</v>
       </c>
+      <c r="E772" t="s">
+        <v>4054</v>
+      </c>
       <c r="F772" t="s">
         <v>3146</v>
       </c>
@@ -34754,6 +34967,9 @@
       <c r="D773" t="s">
         <v>3149</v>
       </c>
+      <c r="E773" t="s">
+        <v>4053</v>
+      </c>
       <c r="F773" t="s">
         <v>3150</v>
       </c>
@@ -34780,6 +34996,9 @@
       <c r="D774" t="s">
         <v>3153</v>
       </c>
+      <c r="E774" t="s">
+        <v>4053</v>
+      </c>
       <c r="F774" t="s">
         <v>3154</v>
       </c>
@@ -34806,6 +35025,9 @@
       <c r="D775" t="s">
         <v>3157</v>
       </c>
+      <c r="E775" t="s">
+        <v>4055</v>
+      </c>
       <c r="F775" t="s">
         <v>3158</v>
       </c>
@@ -34832,6 +35054,9 @@
       <c r="D776" t="s">
         <v>3160</v>
       </c>
+      <c r="E776" t="s">
+        <v>4053</v>
+      </c>
       <c r="F776" t="s">
         <v>3161</v>
       </c>
@@ -34858,6 +35083,9 @@
       <c r="D777" t="s">
         <v>3164</v>
       </c>
+      <c r="E777" t="s">
+        <v>4054</v>
+      </c>
       <c r="F777" t="s">
         <v>3165</v>
       </c>
@@ -34884,6 +35112,9 @@
       <c r="D778" t="s">
         <v>3168</v>
       </c>
+      <c r="E778" t="s">
+        <v>4053</v>
+      </c>
       <c r="F778" t="s">
         <v>3169</v>
       </c>
@@ -34910,6 +35141,9 @@
       <c r="D779" t="s">
         <v>3171</v>
       </c>
+      <c r="E779" t="s">
+        <v>4053</v>
+      </c>
       <c r="F779" t="s">
         <v>3172</v>
       </c>
@@ -34936,6 +35170,9 @@
       <c r="D780" t="s">
         <v>3175</v>
       </c>
+      <c r="E780" t="s">
+        <v>4053</v>
+      </c>
       <c r="F780" t="s">
         <v>3176</v>
       </c>
@@ -34962,6 +35199,9 @@
       <c r="D781" t="s">
         <v>3179</v>
       </c>
+      <c r="E781" t="s">
+        <v>4053</v>
+      </c>
       <c r="F781" t="s">
         <v>3180</v>
       </c>
@@ -34988,6 +35228,9 @@
       <c r="D782" t="s">
         <v>3183</v>
       </c>
+      <c r="E782" t="s">
+        <v>4054</v>
+      </c>
       <c r="F782" t="s">
         <v>3184</v>
       </c>
@@ -35014,6 +35257,9 @@
       <c r="D783" t="s">
         <v>3186</v>
       </c>
+      <c r="E783" t="s">
+        <v>4054</v>
+      </c>
       <c r="F783" t="s">
         <v>3187</v>
       </c>
@@ -35040,6 +35286,9 @@
       <c r="D784" t="s">
         <v>3190</v>
       </c>
+      <c r="E784" t="s">
+        <v>4053</v>
+      </c>
       <c r="F784" t="s">
         <v>3191</v>
       </c>
@@ -35066,6 +35315,9 @@
       <c r="D785" t="s">
         <v>3194</v>
       </c>
+      <c r="E785" t="s">
+        <v>4053</v>
+      </c>
       <c r="F785" t="s">
         <v>3195</v>
       </c>
@@ -35092,6 +35344,9 @@
       <c r="D786" t="s">
         <v>3198</v>
       </c>
+      <c r="E786" t="s">
+        <v>4053</v>
+      </c>
       <c r="F786" t="s">
         <v>3199</v>
       </c>
@@ -35118,6 +35373,9 @@
       <c r="D787" t="s">
         <v>3202</v>
       </c>
+      <c r="E787" t="s">
+        <v>4054</v>
+      </c>
       <c r="F787" t="s">
         <v>3203</v>
       </c>
@@ -35144,6 +35402,9 @@
       <c r="D788" t="s">
         <v>3205</v>
       </c>
+      <c r="E788" t="s">
+        <v>4053</v>
+      </c>
       <c r="F788" t="s">
         <v>3206</v>
       </c>
@@ -35170,6 +35431,9 @@
       <c r="D789" t="s">
         <v>3209</v>
       </c>
+      <c r="E789" t="s">
+        <v>4053</v>
+      </c>
       <c r="F789" t="s">
         <v>3210</v>
       </c>
@@ -35196,6 +35460,9 @@
       <c r="D790" t="s">
         <v>3213</v>
       </c>
+      <c r="E790" t="s">
+        <v>4053</v>
+      </c>
       <c r="F790" t="s">
         <v>3214</v>
       </c>
@@ -35222,6 +35489,9 @@
       <c r="D791" t="s">
         <v>3217</v>
       </c>
+      <c r="E791" t="s">
+        <v>4053</v>
+      </c>
       <c r="F791" t="s">
         <v>3218</v>
       </c>
@@ -35248,6 +35518,9 @@
       <c r="D792" t="s">
         <v>3221</v>
       </c>
+      <c r="E792" t="s">
+        <v>4055</v>
+      </c>
       <c r="F792" t="s">
         <v>3222</v>
       </c>
@@ -35274,6 +35547,9 @@
       <c r="D793" t="s">
         <v>3225</v>
       </c>
+      <c r="E793" t="s">
+        <v>4054</v>
+      </c>
       <c r="F793" t="s">
         <v>3226</v>
       </c>
@@ -35300,6 +35576,9 @@
       <c r="D794" t="s">
         <v>3229</v>
       </c>
+      <c r="E794" t="s">
+        <v>4054</v>
+      </c>
       <c r="F794" t="s">
         <v>3230</v>
       </c>
@@ -35326,6 +35605,9 @@
       <c r="D795" t="s">
         <v>3233</v>
       </c>
+      <c r="E795" t="s">
+        <v>4054</v>
+      </c>
       <c r="F795" t="s">
         <v>3234</v>
       </c>
@@ -35352,6 +35634,9 @@
       <c r="D796" t="s">
         <v>3237</v>
       </c>
+      <c r="E796" t="s">
+        <v>4053</v>
+      </c>
       <c r="F796" t="s">
         <v>3238</v>
       </c>
@@ -35378,6 +35663,9 @@
       <c r="D797" t="s">
         <v>3241</v>
       </c>
+      <c r="E797" t="s">
+        <v>4053</v>
+      </c>
       <c r="F797" t="s">
         <v>3242</v>
       </c>
@@ -35404,6 +35692,9 @@
       <c r="D798" t="s">
         <v>3245</v>
       </c>
+      <c r="E798" t="s">
+        <v>4053</v>
+      </c>
       <c r="F798" t="s">
         <v>3246</v>
       </c>
@@ -35430,6 +35721,9 @@
       <c r="D799" t="s">
         <v>3249</v>
       </c>
+      <c r="E799" t="s">
+        <v>4053</v>
+      </c>
       <c r="F799" t="s">
         <v>3250</v>
       </c>
@@ -35456,6 +35750,9 @@
       <c r="D800" t="s">
         <v>3253</v>
       </c>
+      <c r="E800" t="s">
+        <v>4053</v>
+      </c>
       <c r="F800" t="s">
         <v>3254</v>
       </c>
@@ -35482,6 +35779,9 @@
       <c r="D801" t="s">
         <v>3257</v>
       </c>
+      <c r="E801" t="s">
+        <v>4053</v>
+      </c>
       <c r="F801" t="s">
         <v>3258</v>
       </c>
@@ -35508,6 +35808,9 @@
       <c r="D802" t="s">
         <v>3261</v>
       </c>
+      <c r="E802" t="s">
+        <v>4053</v>
+      </c>
       <c r="F802" t="s">
         <v>3262</v>
       </c>
@@ -35534,6 +35837,9 @@
       <c r="D803" t="s">
         <v>3265</v>
       </c>
+      <c r="E803" t="s">
+        <v>4053</v>
+      </c>
       <c r="F803" t="s">
         <v>3266</v>
       </c>
@@ -35560,6 +35866,9 @@
       <c r="D804" t="s">
         <v>3269</v>
       </c>
+      <c r="E804" t="s">
+        <v>4054</v>
+      </c>
       <c r="F804" t="s">
         <v>3270</v>
       </c>
@@ -35586,6 +35895,9 @@
       <c r="D805" t="s">
         <v>3273</v>
       </c>
+      <c r="E805" t="s">
+        <v>4053</v>
+      </c>
       <c r="F805" t="s">
         <v>3274</v>
       </c>
@@ -35612,6 +35924,9 @@
       <c r="D806" t="s">
         <v>3277</v>
       </c>
+      <c r="E806" t="s">
+        <v>4053</v>
+      </c>
       <c r="F806" t="s">
         <v>3278</v>
       </c>
@@ -35638,6 +35953,9 @@
       <c r="D807" t="s">
         <v>3281</v>
       </c>
+      <c r="E807" t="s">
+        <v>4056</v>
+      </c>
       <c r="F807" t="s">
         <v>3282</v>
       </c>
@@ -35664,6 +35982,9 @@
       <c r="D808" t="s">
         <v>3285</v>
       </c>
+      <c r="E808" t="s">
+        <v>4054</v>
+      </c>
       <c r="F808" t="s">
         <v>3286</v>
       </c>
@@ -35690,6 +36011,9 @@
       <c r="D809" t="s">
         <v>3289</v>
       </c>
+      <c r="E809" t="s">
+        <v>4053</v>
+      </c>
       <c r="F809" t="s">
         <v>3290</v>
       </c>
@@ -35716,6 +36040,9 @@
       <c r="D810" t="s">
         <v>3293</v>
       </c>
+      <c r="E810" t="s">
+        <v>4053</v>
+      </c>
       <c r="F810" t="s">
         <v>3294</v>
       </c>
@@ -35742,6 +36069,9 @@
       <c r="D811" t="s">
         <v>3297</v>
       </c>
+      <c r="E811" t="s">
+        <v>4054</v>
+      </c>
       <c r="F811" t="s">
         <v>3298</v>
       </c>
@@ -35768,6 +36098,9 @@
       <c r="D812" t="s">
         <v>3301</v>
       </c>
+      <c r="E812" t="s">
+        <v>4053</v>
+      </c>
       <c r="F812" t="s">
         <v>3302</v>
       </c>
@@ -35794,6 +36127,9 @@
       <c r="D813" t="s">
         <v>3305</v>
       </c>
+      <c r="E813" t="s">
+        <v>4053</v>
+      </c>
       <c r="F813" t="s">
         <v>3306</v>
       </c>
@@ -35820,6 +36156,9 @@
       <c r="D814" t="s">
         <v>3309</v>
       </c>
+      <c r="E814" t="s">
+        <v>4053</v>
+      </c>
       <c r="F814" t="s">
         <v>3310</v>
       </c>
@@ -35846,6 +36185,9 @@
       <c r="D815" t="s">
         <v>3313</v>
       </c>
+      <c r="E815" t="s">
+        <v>4056</v>
+      </c>
       <c r="F815" t="s">
         <v>3314</v>
       </c>
@@ -35872,6 +36214,9 @@
       <c r="D816" t="s">
         <v>3317</v>
       </c>
+      <c r="E816" t="s">
+        <v>4053</v>
+      </c>
       <c r="F816" t="s">
         <v>3318</v>
       </c>
@@ -35898,6 +36243,9 @@
       <c r="D817" t="s">
         <v>3321</v>
       </c>
+      <c r="E817" t="s">
+        <v>4054</v>
+      </c>
       <c r="F817" t="s">
         <v>3322</v>
       </c>
@@ -35924,6 +36272,9 @@
       <c r="D818" t="s">
         <v>3325</v>
       </c>
+      <c r="E818" t="s">
+        <v>4053</v>
+      </c>
       <c r="F818" t="s">
         <v>3326</v>
       </c>
@@ -35950,6 +36301,9 @@
       <c r="D819" t="s">
         <v>3329</v>
       </c>
+      <c r="E819" t="s">
+        <v>4054</v>
+      </c>
       <c r="F819" t="s">
         <v>3330</v>
       </c>
@@ -35976,6 +36330,9 @@
       <c r="D820" t="s">
         <v>3333</v>
       </c>
+      <c r="E820" t="s">
+        <v>4054</v>
+      </c>
       <c r="F820" t="s">
         <v>3334</v>
       </c>
@@ -36002,6 +36359,9 @@
       <c r="D821" t="s">
         <v>3337</v>
       </c>
+      <c r="E821" t="s">
+        <v>4053</v>
+      </c>
       <c r="F821" t="s">
         <v>3338</v>
       </c>
@@ -36028,6 +36388,9 @@
       <c r="D822" t="s">
         <v>3341</v>
       </c>
+      <c r="E822" t="s">
+        <v>4055</v>
+      </c>
       <c r="F822" t="s">
         <v>3342</v>
       </c>
@@ -36054,6 +36417,9 @@
       <c r="D823" t="s">
         <v>3345</v>
       </c>
+      <c r="E823" t="s">
+        <v>4053</v>
+      </c>
       <c r="F823" t="s">
         <v>3346</v>
       </c>
@@ -36080,6 +36446,9 @@
       <c r="D824" t="s">
         <v>3349</v>
       </c>
+      <c r="E824" t="s">
+        <v>4053</v>
+      </c>
       <c r="F824" t="s">
         <v>3350</v>
       </c>
@@ -36106,6 +36475,9 @@
       <c r="D825" t="s">
         <v>3352</v>
       </c>
+      <c r="E825" t="s">
+        <v>4056</v>
+      </c>
       <c r="F825" t="s">
         <v>3353</v>
       </c>
@@ -36132,6 +36504,9 @@
       <c r="D826" t="s">
         <v>3356</v>
       </c>
+      <c r="E826" t="s">
+        <v>4053</v>
+      </c>
       <c r="F826" t="s">
         <v>3357</v>
       </c>
@@ -36158,6 +36533,9 @@
       <c r="D827" t="s">
         <v>3360</v>
       </c>
+      <c r="E827" t="s">
+        <v>4054</v>
+      </c>
       <c r="F827" t="s">
         <v>3361</v>
       </c>
@@ -36184,6 +36562,9 @@
       <c r="D828" t="s">
         <v>3364</v>
       </c>
+      <c r="E828" t="s">
+        <v>4053</v>
+      </c>
       <c r="F828" t="s">
         <v>3365</v>
       </c>
@@ -36210,6 +36591,9 @@
       <c r="D829" t="s">
         <v>3367</v>
       </c>
+      <c r="E829" t="s">
+        <v>4054</v>
+      </c>
       <c r="F829" t="s">
         <v>3368</v>
       </c>
@@ -36236,6 +36620,9 @@
       <c r="D830" t="s">
         <v>3371</v>
       </c>
+      <c r="E830" t="s">
+        <v>4054</v>
+      </c>
       <c r="F830" t="s">
         <v>3372</v>
       </c>
@@ -36262,6 +36649,9 @@
       <c r="D831" t="s">
         <v>3375</v>
       </c>
+      <c r="E831" t="s">
+        <v>4055</v>
+      </c>
       <c r="F831" t="s">
         <v>3376</v>
       </c>
@@ -36288,6 +36678,9 @@
       <c r="D832" t="s">
         <v>3379</v>
       </c>
+      <c r="E832" t="s">
+        <v>4053</v>
+      </c>
       <c r="F832" t="s">
         <v>3380</v>
       </c>
@@ -36314,6 +36707,9 @@
       <c r="D833" t="s">
         <v>3383</v>
       </c>
+      <c r="E833" t="s">
+        <v>4053</v>
+      </c>
       <c r="F833" t="s">
         <v>3384</v>
       </c>
@@ -36340,6 +36736,9 @@
       <c r="D834" t="s">
         <v>3387</v>
       </c>
+      <c r="E834" t="s">
+        <v>4053</v>
+      </c>
       <c r="F834" t="s">
         <v>3388</v>
       </c>
@@ -36366,6 +36765,9 @@
       <c r="D835" t="s">
         <v>3391</v>
       </c>
+      <c r="E835" t="s">
+        <v>4053</v>
+      </c>
       <c r="F835" t="s">
         <v>3392</v>
       </c>
@@ -36392,6 +36794,9 @@
       <c r="D836" t="s">
         <v>3395</v>
       </c>
+      <c r="E836" t="s">
+        <v>4053</v>
+      </c>
       <c r="F836" t="s">
         <v>3396</v>
       </c>
@@ -36418,6 +36823,9 @@
       <c r="D837" t="s">
         <v>3399</v>
       </c>
+      <c r="E837" t="s">
+        <v>4054</v>
+      </c>
       <c r="F837" t="s">
         <v>3400</v>
       </c>
@@ -36444,6 +36852,9 @@
       <c r="D838" t="s">
         <v>3403</v>
       </c>
+      <c r="E838" t="s">
+        <v>4053</v>
+      </c>
       <c r="F838" t="s">
         <v>3404</v>
       </c>
@@ -36470,6 +36881,9 @@
       <c r="D839" t="s">
         <v>3407</v>
       </c>
+      <c r="E839" t="s">
+        <v>4053</v>
+      </c>
       <c r="F839" t="s">
         <v>3408</v>
       </c>
@@ -36496,6 +36910,9 @@
       <c r="D840" t="s">
         <v>3412</v>
       </c>
+      <c r="E840" t="s">
+        <v>4056</v>
+      </c>
       <c r="F840" t="s">
         <v>3413</v>
       </c>
@@ -36522,6 +36939,9 @@
       <c r="D841" t="s">
         <v>3416</v>
       </c>
+      <c r="E841" t="s">
+        <v>4054</v>
+      </c>
       <c r="F841" t="s">
         <v>3417</v>
       </c>
@@ -36548,6 +36968,9 @@
       <c r="D842" t="s">
         <v>3420</v>
       </c>
+      <c r="E842" t="s">
+        <v>4053</v>
+      </c>
       <c r="F842" t="s">
         <v>3421</v>
       </c>
@@ -36574,6 +36997,9 @@
       <c r="D843" t="s">
         <v>3424</v>
       </c>
+      <c r="E843" t="s">
+        <v>4053</v>
+      </c>
       <c r="F843" t="s">
         <v>3425</v>
       </c>
@@ -36600,6 +37026,9 @@
       <c r="D844" t="s">
         <v>3428</v>
       </c>
+      <c r="E844" t="s">
+        <v>4054</v>
+      </c>
       <c r="F844" t="s">
         <v>3429</v>
       </c>
@@ -36626,6 +37055,9 @@
       <c r="D845" t="s">
         <v>3432</v>
       </c>
+      <c r="E845" t="s">
+        <v>4053</v>
+      </c>
       <c r="F845" t="s">
         <v>3433</v>
       </c>
@@ -36652,6 +37084,9 @@
       <c r="D846" t="s">
         <v>3436</v>
       </c>
+      <c r="E846" t="s">
+        <v>4054</v>
+      </c>
       <c r="F846" t="s">
         <v>3437</v>
       </c>
@@ -36678,6 +37113,9 @@
       <c r="D847" t="s">
         <v>3440</v>
       </c>
+      <c r="E847" t="s">
+        <v>4054</v>
+      </c>
       <c r="F847" t="s">
         <v>3441</v>
       </c>
@@ -36704,6 +37142,9 @@
       <c r="D848" t="s">
         <v>3444</v>
       </c>
+      <c r="E848" t="s">
+        <v>4053</v>
+      </c>
       <c r="F848" t="s">
         <v>3445</v>
       </c>
@@ -36730,6 +37171,9 @@
       <c r="D849" t="s">
         <v>3448</v>
       </c>
+      <c r="E849" t="s">
+        <v>4053</v>
+      </c>
       <c r="F849" t="s">
         <v>3449</v>
       </c>
@@ -36756,6 +37200,9 @@
       <c r="D850" t="s">
         <v>3452</v>
       </c>
+      <c r="E850" t="s">
+        <v>4054</v>
+      </c>
       <c r="F850" t="s">
         <v>3453</v>
       </c>
@@ -36782,6 +37229,9 @@
       <c r="D851" t="s">
         <v>3456</v>
       </c>
+      <c r="E851" t="s">
+        <v>4053</v>
+      </c>
       <c r="F851" t="s">
         <v>3457</v>
       </c>
@@ -36808,6 +37258,9 @@
       <c r="D852" t="s">
         <v>3460</v>
       </c>
+      <c r="E852" t="s">
+        <v>4053</v>
+      </c>
       <c r="F852" t="s">
         <v>3461</v>
       </c>
@@ -36834,6 +37287,9 @@
       <c r="D853" t="s">
         <v>3464</v>
       </c>
+      <c r="E853" t="s">
+        <v>4053</v>
+      </c>
       <c r="F853" t="s">
         <v>3465</v>
       </c>
@@ -36860,6 +37316,9 @@
       <c r="D854" t="s">
         <v>3468</v>
       </c>
+      <c r="E854" t="s">
+        <v>4053</v>
+      </c>
       <c r="F854" t="s">
         <v>3469</v>
       </c>
@@ -36886,6 +37345,9 @@
       <c r="D855" t="s">
         <v>3472</v>
       </c>
+      <c r="E855" t="s">
+        <v>4053</v>
+      </c>
       <c r="F855" t="s">
         <v>3473</v>
       </c>
@@ -36912,6 +37374,9 @@
       <c r="D856" t="s">
         <v>3476</v>
       </c>
+      <c r="E856" t="s">
+        <v>4054</v>
+      </c>
       <c r="F856" t="s">
         <v>3477</v>
       </c>
@@ -36938,6 +37403,9 @@
       <c r="D857" t="s">
         <v>3480</v>
       </c>
+      <c r="E857" t="s">
+        <v>4054</v>
+      </c>
       <c r="F857" t="s">
         <v>3481</v>
       </c>
@@ -36964,6 +37432,9 @@
       <c r="D858" t="s">
         <v>3484</v>
       </c>
+      <c r="E858" t="s">
+        <v>4056</v>
+      </c>
       <c r="F858" t="s">
         <v>3485</v>
       </c>
@@ -36990,6 +37461,9 @@
       <c r="D859" t="s">
         <v>3488</v>
       </c>
+      <c r="E859" t="s">
+        <v>4054</v>
+      </c>
       <c r="F859" t="s">
         <v>3489</v>
       </c>
@@ -37016,6 +37490,9 @@
       <c r="D860" t="s">
         <v>3492</v>
       </c>
+      <c r="E860" t="s">
+        <v>4053</v>
+      </c>
       <c r="F860" t="s">
         <v>3493</v>
       </c>
@@ -37042,6 +37519,9 @@
       <c r="D861" t="s">
         <v>3496</v>
       </c>
+      <c r="E861" t="s">
+        <v>4053</v>
+      </c>
       <c r="F861" t="s">
         <v>3497</v>
       </c>
@@ -37068,6 +37548,9 @@
       <c r="D862" t="s">
         <v>3500</v>
       </c>
+      <c r="E862" t="s">
+        <v>4053</v>
+      </c>
       <c r="F862" t="s">
         <v>3501</v>
       </c>
@@ -37094,6 +37577,9 @@
       <c r="D863" t="s">
         <v>3504</v>
       </c>
+      <c r="E863" t="s">
+        <v>4056</v>
+      </c>
       <c r="F863" t="s">
         <v>3505</v>
       </c>
@@ -37120,6 +37606,9 @@
       <c r="D864" t="s">
         <v>3508</v>
       </c>
+      <c r="E864" t="s">
+        <v>4054</v>
+      </c>
       <c r="F864" t="s">
         <v>3509</v>
       </c>
@@ -37146,6 +37635,9 @@
       <c r="D865" t="s">
         <v>3512</v>
       </c>
+      <c r="E865" t="s">
+        <v>4054</v>
+      </c>
       <c r="F865" t="s">
         <v>3513</v>
       </c>
@@ -37172,6 +37664,9 @@
       <c r="D866" t="s">
         <v>3516</v>
       </c>
+      <c r="E866" t="s">
+        <v>4055</v>
+      </c>
       <c r="F866" t="s">
         <v>3517</v>
       </c>
@@ -37198,6 +37693,9 @@
       <c r="D867" t="s">
         <v>3520</v>
       </c>
+      <c r="E867" t="s">
+        <v>4053</v>
+      </c>
       <c r="F867" t="s">
         <v>3521</v>
       </c>
@@ -37224,6 +37722,9 @@
       <c r="D868" t="s">
         <v>3524</v>
       </c>
+      <c r="E868" t="s">
+        <v>4053</v>
+      </c>
       <c r="F868" t="s">
         <v>3525</v>
       </c>
@@ -37250,6 +37751,9 @@
       <c r="D869" t="s">
         <v>3528</v>
       </c>
+      <c r="E869" t="s">
+        <v>4054</v>
+      </c>
       <c r="F869" t="s">
         <v>3529</v>
       </c>
@@ -37276,6 +37780,9 @@
       <c r="D870" t="s">
         <v>3532</v>
       </c>
+      <c r="E870" t="s">
+        <v>4054</v>
+      </c>
       <c r="F870" t="s">
         <v>3533</v>
       </c>
@@ -37302,6 +37809,9 @@
       <c r="D871" t="s">
         <v>3536</v>
       </c>
+      <c r="E871" t="s">
+        <v>4054</v>
+      </c>
       <c r="F871" t="s">
         <v>3537</v>
       </c>
@@ -37328,6 +37838,9 @@
       <c r="D872" t="s">
         <v>3539</v>
       </c>
+      <c r="E872" t="s">
+        <v>4053</v>
+      </c>
       <c r="F872" t="s">
         <v>3540</v>
       </c>
@@ -37354,6 +37867,9 @@
       <c r="D873" t="s">
         <v>3543</v>
       </c>
+      <c r="E873" t="s">
+        <v>4054</v>
+      </c>
       <c r="F873" t="s">
         <v>3544</v>
       </c>
@@ -37380,6 +37896,9 @@
       <c r="D874" t="s">
         <v>3547</v>
       </c>
+      <c r="E874" t="s">
+        <v>4054</v>
+      </c>
       <c r="F874" t="s">
         <v>3548</v>
       </c>
@@ -37406,6 +37925,9 @@
       <c r="D875" t="s">
         <v>3551</v>
       </c>
+      <c r="E875" t="s">
+        <v>4054</v>
+      </c>
       <c r="F875" t="s">
         <v>3552</v>
       </c>
@@ -37432,6 +37954,9 @@
       <c r="D876" t="s">
         <v>3555</v>
       </c>
+      <c r="E876" t="s">
+        <v>4055</v>
+      </c>
       <c r="F876" t="s">
         <v>3556</v>
       </c>
@@ -37458,6 +37983,9 @@
       <c r="D877" t="s">
         <v>3559</v>
       </c>
+      <c r="E877" t="s">
+        <v>4054</v>
+      </c>
       <c r="F877" t="s">
         <v>3560</v>
       </c>
@@ -37484,6 +38012,9 @@
       <c r="D878" t="s">
         <v>3563</v>
       </c>
+      <c r="E878" t="s">
+        <v>4054</v>
+      </c>
       <c r="F878" t="s">
         <v>3564</v>
       </c>
@@ -37510,6 +38041,9 @@
       <c r="D879" t="s">
         <v>3567</v>
       </c>
+      <c r="E879" t="s">
+        <v>4054</v>
+      </c>
       <c r="F879" t="s">
         <v>3568</v>
       </c>
@@ -37536,6 +38070,9 @@
       <c r="D880" t="s">
         <v>3571</v>
       </c>
+      <c r="E880" t="s">
+        <v>4054</v>
+      </c>
       <c r="F880" t="s">
         <v>3572</v>
       </c>
@@ -37562,6 +38099,9 @@
       <c r="D881" t="s">
         <v>3575</v>
       </c>
+      <c r="E881" t="s">
+        <v>4054</v>
+      </c>
       <c r="F881" t="s">
         <v>3576</v>
       </c>
@@ -37588,6 +38128,9 @@
       <c r="D882" t="s">
         <v>3580</v>
       </c>
+      <c r="E882" t="s">
+        <v>4054</v>
+      </c>
       <c r="F882" t="s">
         <v>3581</v>
       </c>
@@ -37614,6 +38157,9 @@
       <c r="D883" t="s">
         <v>3584</v>
       </c>
+      <c r="E883" t="s">
+        <v>4054</v>
+      </c>
       <c r="F883" t="s">
         <v>3585</v>
       </c>
@@ -37640,6 +38186,9 @@
       <c r="D884" t="s">
         <v>3588</v>
       </c>
+      <c r="E884" t="s">
+        <v>4054</v>
+      </c>
       <c r="F884" t="s">
         <v>3589</v>
       </c>
@@ -37666,6 +38215,9 @@
       <c r="D885" t="s">
         <v>3592</v>
       </c>
+      <c r="E885" t="s">
+        <v>4056</v>
+      </c>
       <c r="F885" t="s">
         <v>3593</v>
       </c>
@@ -37692,6 +38244,9 @@
       <c r="D886" t="s">
         <v>3596</v>
       </c>
+      <c r="E886" t="s">
+        <v>4054</v>
+      </c>
       <c r="F886" t="s">
         <v>3597</v>
       </c>
@@ -37718,6 +38273,9 @@
       <c r="D887" t="s">
         <v>3600</v>
       </c>
+      <c r="E887" t="s">
+        <v>4054</v>
+      </c>
       <c r="F887" t="s">
         <v>3601</v>
       </c>
@@ -37744,6 +38302,9 @@
       <c r="D888" t="s">
         <v>3604</v>
       </c>
+      <c r="E888" t="s">
+        <v>4054</v>
+      </c>
       <c r="F888" t="s">
         <v>3605</v>
       </c>
@@ -37770,6 +38331,9 @@
       <c r="D889" t="s">
         <v>3608</v>
       </c>
+      <c r="E889" t="s">
+        <v>4054</v>
+      </c>
       <c r="F889" t="s">
         <v>3609</v>
       </c>
@@ -37796,6 +38360,9 @@
       <c r="D890" t="s">
         <v>3612</v>
       </c>
+      <c r="E890" t="s">
+        <v>4054</v>
+      </c>
       <c r="F890" t="s">
         <v>3613</v>
       </c>
@@ -37822,6 +38389,9 @@
       <c r="D891" t="s">
         <v>3616</v>
       </c>
+      <c r="E891" t="s">
+        <v>4053</v>
+      </c>
       <c r="F891" t="s">
         <v>3617</v>
       </c>
@@ -37848,6 +38418,9 @@
       <c r="D892" t="s">
         <v>3620</v>
       </c>
+      <c r="E892" t="s">
+        <v>4054</v>
+      </c>
       <c r="F892" t="s">
         <v>3621</v>
       </c>
@@ -37874,6 +38447,9 @@
       <c r="D893" t="s">
         <v>3624</v>
       </c>
+      <c r="E893" t="s">
+        <v>4054</v>
+      </c>
       <c r="F893" t="s">
         <v>3625</v>
       </c>
@@ -37900,6 +38476,9 @@
       <c r="D894" t="s">
         <v>3628</v>
       </c>
+      <c r="E894" t="s">
+        <v>4054</v>
+      </c>
       <c r="F894" t="s">
         <v>3629</v>
       </c>
@@ -37926,6 +38505,9 @@
       <c r="D895" t="s">
         <v>3632</v>
       </c>
+      <c r="E895" t="s">
+        <v>4053</v>
+      </c>
       <c r="F895" t="s">
         <v>3633</v>
       </c>
@@ -37952,6 +38534,9 @@
       <c r="D896" t="s">
         <v>3636</v>
       </c>
+      <c r="E896" t="s">
+        <v>4053</v>
+      </c>
       <c r="F896" t="s">
         <v>3637</v>
       </c>
@@ -37978,6 +38563,9 @@
       <c r="D897" t="s">
         <v>3640</v>
       </c>
+      <c r="E897" t="s">
+        <v>4054</v>
+      </c>
       <c r="F897" t="s">
         <v>3641</v>
       </c>
@@ -38004,6 +38592,9 @@
       <c r="D898" t="s">
         <v>3644</v>
       </c>
+      <c r="E898" t="s">
+        <v>4053</v>
+      </c>
       <c r="F898" t="s">
         <v>3645</v>
       </c>
@@ -38030,6 +38621,9 @@
       <c r="D899" t="s">
         <v>3648</v>
       </c>
+      <c r="E899" t="s">
+        <v>4053</v>
+      </c>
       <c r="F899" t="s">
         <v>3649</v>
       </c>
@@ -38056,6 +38650,9 @@
       <c r="D900" t="s">
         <v>3652</v>
       </c>
+      <c r="E900" t="s">
+        <v>4053</v>
+      </c>
       <c r="F900" t="s">
         <v>3653</v>
       </c>
@@ -38082,6 +38679,9 @@
       <c r="D901" t="s">
         <v>3656</v>
       </c>
+      <c r="E901" t="s">
+        <v>4053</v>
+      </c>
       <c r="F901" t="s">
         <v>3657</v>
       </c>
@@ -38108,6 +38708,9 @@
       <c r="D902" t="s">
         <v>3660</v>
       </c>
+      <c r="E902" t="s">
+        <v>4053</v>
+      </c>
       <c r="F902" t="s">
         <v>3661</v>
       </c>
@@ -38134,6 +38737,9 @@
       <c r="D903" t="s">
         <v>3664</v>
       </c>
+      <c r="E903" t="s">
+        <v>4054</v>
+      </c>
       <c r="F903" t="s">
         <v>3665</v>
       </c>
@@ -38160,6 +38766,9 @@
       <c r="D904" t="s">
         <v>3668</v>
       </c>
+      <c r="E904" t="s">
+        <v>4053</v>
+      </c>
       <c r="F904" t="s">
         <v>3669</v>
       </c>
@@ -38186,6 +38795,9 @@
       <c r="D905" t="s">
         <v>3672</v>
       </c>
+      <c r="E905" t="s">
+        <v>4054</v>
+      </c>
       <c r="F905" t="s">
         <v>3673</v>
       </c>
@@ -38212,6 +38824,9 @@
       <c r="D906" t="s">
         <v>3676</v>
       </c>
+      <c r="E906" t="s">
+        <v>4053</v>
+      </c>
       <c r="F906" t="s">
         <v>3677</v>
       </c>
@@ -38238,6 +38853,9 @@
       <c r="D907" t="s">
         <v>3680</v>
       </c>
+      <c r="E907" t="s">
+        <v>4053</v>
+      </c>
       <c r="F907" t="s">
         <v>3681</v>
       </c>
@@ -38264,6 +38882,9 @@
       <c r="D908" t="s">
         <v>3685</v>
       </c>
+      <c r="E908" t="s">
+        <v>4053</v>
+      </c>
       <c r="F908" t="s">
         <v>3686</v>
       </c>
@@ -38290,6 +38911,9 @@
       <c r="D909" t="s">
         <v>3689</v>
       </c>
+      <c r="E909" t="s">
+        <v>4054</v>
+      </c>
       <c r="F909" t="s">
         <v>3690</v>
       </c>
@@ -38316,6 +38940,9 @@
       <c r="D910" t="s">
         <v>3693</v>
       </c>
+      <c r="E910" t="s">
+        <v>4055</v>
+      </c>
       <c r="F910" t="s">
         <v>3694</v>
       </c>
@@ -38342,6 +38969,9 @@
       <c r="D911" t="s">
         <v>3697</v>
       </c>
+      <c r="E911" t="s">
+        <v>4053</v>
+      </c>
       <c r="F911" t="s">
         <v>3698</v>
       </c>
@@ -38368,6 +38998,9 @@
       <c r="D912" t="s">
         <v>3701</v>
       </c>
+      <c r="E912" t="s">
+        <v>4054</v>
+      </c>
       <c r="F912" t="s">
         <v>3702</v>
       </c>
@@ -38394,6 +39027,9 @@
       <c r="D913" t="s">
         <v>3705</v>
       </c>
+      <c r="E913" t="s">
+        <v>4055</v>
+      </c>
       <c r="F913" t="s">
         <v>3706</v>
       </c>
@@ -38420,6 +39056,9 @@
       <c r="D914" t="s">
         <v>3709</v>
       </c>
+      <c r="E914" t="s">
+        <v>4053</v>
+      </c>
       <c r="F914" t="s">
         <v>3710</v>
       </c>
@@ -38446,6 +39085,9 @@
       <c r="D915" t="s">
         <v>3713</v>
       </c>
+      <c r="E915" t="s">
+        <v>4053</v>
+      </c>
       <c r="F915" t="s">
         <v>3714</v>
       </c>
@@ -38472,6 +39114,9 @@
       <c r="D916" t="s">
         <v>3717</v>
       </c>
+      <c r="E916" t="s">
+        <v>4054</v>
+      </c>
       <c r="F916" t="s">
         <v>3718</v>
       </c>
@@ -38498,6 +39143,9 @@
       <c r="D917" t="s">
         <v>3721</v>
       </c>
+      <c r="E917" t="s">
+        <v>4053</v>
+      </c>
       <c r="F917" t="s">
         <v>3722</v>
       </c>
@@ -38524,6 +39172,9 @@
       <c r="D918" t="s">
         <v>3725</v>
       </c>
+      <c r="E918" t="s">
+        <v>4054</v>
+      </c>
       <c r="F918" t="s">
         <v>3726</v>
       </c>
@@ -38550,6 +39201,9 @@
       <c r="D919" t="s">
         <v>3729</v>
       </c>
+      <c r="E919" t="s">
+        <v>4056</v>
+      </c>
       <c r="F919" t="s">
         <v>3730</v>
       </c>
@@ -38576,6 +39230,9 @@
       <c r="D920" t="s">
         <v>3733</v>
       </c>
+      <c r="E920" t="s">
+        <v>4053</v>
+      </c>
       <c r="F920" t="s">
         <v>3734</v>
       </c>
@@ -38602,6 +39259,9 @@
       <c r="D921" t="s">
         <v>3737</v>
       </c>
+      <c r="E921" t="s">
+        <v>4054</v>
+      </c>
       <c r="F921" t="s">
         <v>3738</v>
       </c>
@@ -38628,6 +39288,9 @@
       <c r="D922" t="s">
         <v>3741</v>
       </c>
+      <c r="E922" t="s">
+        <v>4054</v>
+      </c>
       <c r="F922" t="s">
         <v>3742</v>
       </c>
@@ -38654,6 +39317,9 @@
       <c r="D923" t="s">
         <v>3745</v>
       </c>
+      <c r="E923" t="s">
+        <v>4053</v>
+      </c>
       <c r="F923" t="s">
         <v>3746</v>
       </c>
@@ -38680,6 +39346,9 @@
       <c r="D924" t="s">
         <v>3749</v>
       </c>
+      <c r="E924" t="s">
+        <v>4053</v>
+      </c>
       <c r="F924" t="s">
         <v>3750</v>
       </c>
@@ -38706,6 +39375,9 @@
       <c r="D925" t="s">
         <v>3753</v>
       </c>
+      <c r="E925" t="s">
+        <v>4056</v>
+      </c>
       <c r="F925" t="s">
         <v>3754</v>
       </c>
@@ -38732,6 +39404,9 @@
       <c r="D926" t="s">
         <v>3757</v>
       </c>
+      <c r="E926" t="s">
+        <v>4053</v>
+      </c>
       <c r="F926" t="s">
         <v>3758</v>
       </c>
@@ -38758,6 +39433,9 @@
       <c r="D927" t="s">
         <v>3761</v>
       </c>
+      <c r="E927" t="s">
+        <v>4054</v>
+      </c>
       <c r="F927" t="s">
         <v>3762</v>
       </c>
@@ -38784,6 +39462,9 @@
       <c r="D928" t="s">
         <v>3765</v>
       </c>
+      <c r="E928" t="s">
+        <v>4054</v>
+      </c>
       <c r="F928" t="s">
         <v>3766</v>
       </c>
@@ -38810,6 +39491,9 @@
       <c r="D929" t="s">
         <v>3769</v>
       </c>
+      <c r="E929" t="s">
+        <v>4054</v>
+      </c>
       <c r="F929" t="s">
         <v>3770</v>
       </c>
@@ -38836,6 +39520,9 @@
       <c r="D930" t="s">
         <v>3773</v>
       </c>
+      <c r="E930" t="s">
+        <v>4053</v>
+      </c>
       <c r="F930" t="s">
         <v>3774</v>
       </c>
@@ -38862,6 +39549,9 @@
       <c r="D931" t="s">
         <v>3777</v>
       </c>
+      <c r="E931" t="s">
+        <v>4053</v>
+      </c>
       <c r="F931" t="s">
         <v>3778</v>
       </c>
@@ -38888,6 +39578,9 @@
       <c r="D932" t="s">
         <v>3781</v>
       </c>
+      <c r="E932" t="s">
+        <v>4054</v>
+      </c>
       <c r="F932" t="s">
         <v>3782</v>
       </c>
@@ -38914,6 +39607,9 @@
       <c r="D933" t="s">
         <v>3785</v>
       </c>
+      <c r="E933" t="s">
+        <v>4054</v>
+      </c>
       <c r="F933" t="s">
         <v>3786</v>
       </c>
@@ -38940,6 +39636,9 @@
       <c r="D934" t="s">
         <v>3789</v>
       </c>
+      <c r="E934" t="s">
+        <v>4053</v>
+      </c>
       <c r="F934" t="s">
         <v>3790</v>
       </c>
@@ -38966,6 +39665,9 @@
       <c r="D935" t="s">
         <v>3793</v>
       </c>
+      <c r="E935" t="s">
+        <v>4053</v>
+      </c>
       <c r="F935" t="s">
         <v>3794</v>
       </c>
@@ -38992,6 +39694,9 @@
       <c r="D936" t="s">
         <v>3797</v>
       </c>
+      <c r="E936" t="s">
+        <v>4053</v>
+      </c>
       <c r="F936" t="s">
         <v>3798</v>
       </c>
@@ -39018,6 +39723,9 @@
       <c r="D937" t="s">
         <v>3801</v>
       </c>
+      <c r="E937" t="s">
+        <v>4054</v>
+      </c>
       <c r="F937" t="s">
         <v>3802</v>
       </c>
@@ -39044,6 +39752,9 @@
       <c r="D938" t="s">
         <v>3805</v>
       </c>
+      <c r="E938" t="s">
+        <v>4053</v>
+      </c>
       <c r="F938" t="s">
         <v>3806</v>
       </c>
@@ -39070,6 +39781,9 @@
       <c r="D939" t="s">
         <v>3809</v>
       </c>
+      <c r="E939" t="s">
+        <v>4054</v>
+      </c>
       <c r="F939" t="s">
         <v>3810</v>
       </c>
@@ -39096,6 +39810,9 @@
       <c r="D940" t="s">
         <v>3813</v>
       </c>
+      <c r="E940" t="s">
+        <v>4053</v>
+      </c>
       <c r="F940" t="s">
         <v>3814</v>
       </c>
@@ -39122,6 +39839,9 @@
       <c r="D941" t="s">
         <v>3817</v>
       </c>
+      <c r="E941" t="s">
+        <v>4054</v>
+      </c>
       <c r="F941" t="s">
         <v>3818</v>
       </c>
@@ -39148,6 +39868,9 @@
       <c r="D942" t="s">
         <v>3821</v>
       </c>
+      <c r="E942" t="s">
+        <v>4054</v>
+      </c>
       <c r="F942" t="s">
         <v>3822</v>
       </c>
@@ -39174,6 +39897,9 @@
       <c r="D943" t="s">
         <v>3825</v>
       </c>
+      <c r="E943" t="s">
+        <v>4054</v>
+      </c>
       <c r="F943" t="s">
         <v>3826</v>
       </c>
@@ -39200,6 +39926,9 @@
       <c r="D944" t="s">
         <v>3829</v>
       </c>
+      <c r="E944" t="s">
+        <v>4053</v>
+      </c>
       <c r="F944" t="s">
         <v>3830</v>
       </c>
@@ -39226,6 +39955,9 @@
       <c r="D945" t="s">
         <v>3833</v>
       </c>
+      <c r="E945" t="s">
+        <v>4053</v>
+      </c>
       <c r="F945" t="s">
         <v>3834</v>
       </c>
@@ -39252,6 +39984,9 @@
       <c r="D946" t="s">
         <v>3837</v>
       </c>
+      <c r="E946" t="s">
+        <v>4053</v>
+      </c>
       <c r="F946" t="s">
         <v>3838</v>
       </c>
@@ -39278,6 +40013,9 @@
       <c r="D947" t="s">
         <v>3841</v>
       </c>
+      <c r="E947" t="s">
+        <v>4053</v>
+      </c>
       <c r="F947" t="s">
         <v>3842</v>
       </c>
@@ -39304,6 +40042,9 @@
       <c r="D948" t="s">
         <v>3845</v>
       </c>
+      <c r="E948" t="s">
+        <v>4053</v>
+      </c>
       <c r="F948" t="s">
         <v>3846</v>
       </c>
@@ -39330,6 +40071,9 @@
       <c r="D949" t="s">
         <v>3849</v>
       </c>
+      <c r="E949" t="s">
+        <v>4053</v>
+      </c>
       <c r="F949" t="s">
         <v>3850</v>
       </c>
@@ -39356,6 +40100,9 @@
       <c r="D950" t="s">
         <v>3853</v>
       </c>
+      <c r="E950" t="s">
+        <v>4053</v>
+      </c>
       <c r="F950" t="s">
         <v>3854</v>
       </c>
@@ -39382,6 +40129,9 @@
       <c r="D951" t="s">
         <v>3857</v>
       </c>
+      <c r="E951" t="s">
+        <v>4054</v>
+      </c>
       <c r="F951" t="s">
         <v>3858</v>
       </c>
@@ -39408,6 +40158,9 @@
       <c r="D952" t="s">
         <v>3861</v>
       </c>
+      <c r="E952" t="s">
+        <v>4054</v>
+      </c>
       <c r="F952" t="s">
         <v>3862</v>
       </c>
@@ -39434,6 +40187,9 @@
       <c r="D953" t="s">
         <v>3865</v>
       </c>
+      <c r="E953" t="s">
+        <v>4053</v>
+      </c>
       <c r="F953" t="s">
         <v>3866</v>
       </c>
@@ -39460,6 +40216,9 @@
       <c r="D954" t="s">
         <v>3869</v>
       </c>
+      <c r="E954" t="s">
+        <v>4056</v>
+      </c>
       <c r="F954" t="s">
         <v>3870</v>
       </c>
@@ -39486,6 +40245,9 @@
       <c r="D955" t="s">
         <v>3872</v>
       </c>
+      <c r="E955" t="s">
+        <v>4054</v>
+      </c>
       <c r="F955" t="s">
         <v>3873</v>
       </c>
@@ -39512,6 +40274,9 @@
       <c r="D956" t="s">
         <v>3876</v>
       </c>
+      <c r="E956" t="s">
+        <v>4053</v>
+      </c>
       <c r="F956" t="s">
         <v>3877</v>
       </c>
@@ -39538,6 +40303,9 @@
       <c r="D957" t="s">
         <v>3880</v>
       </c>
+      <c r="E957" t="s">
+        <v>4055</v>
+      </c>
       <c r="F957" t="s">
         <v>3881</v>
       </c>
@@ -39564,6 +40332,9 @@
       <c r="D958" t="s">
         <v>3884</v>
       </c>
+      <c r="E958" t="s">
+        <v>4055</v>
+      </c>
       <c r="F958" t="s">
         <v>3885</v>
       </c>
@@ -39590,6 +40361,9 @@
       <c r="D959" t="s">
         <v>3888</v>
       </c>
+      <c r="E959" t="s">
+        <v>4054</v>
+      </c>
       <c r="F959" t="s">
         <v>3889</v>
       </c>
@@ -39616,6 +40390,9 @@
       <c r="D960" t="s">
         <v>3892</v>
       </c>
+      <c r="E960" t="s">
+        <v>4053</v>
+      </c>
       <c r="F960" t="s">
         <v>3893</v>
       </c>
@@ -39642,6 +40419,9 @@
       <c r="D961" t="s">
         <v>3895</v>
       </c>
+      <c r="E961" t="s">
+        <v>4054</v>
+      </c>
       <c r="F961" t="s">
         <v>3896</v>
       </c>
@@ -39668,6 +40448,9 @@
       <c r="D962" t="s">
         <v>3899</v>
       </c>
+      <c r="E962" t="s">
+        <v>4053</v>
+      </c>
       <c r="F962" t="s">
         <v>3900</v>
       </c>
@@ -39694,6 +40477,9 @@
       <c r="D963" t="s">
         <v>3903</v>
       </c>
+      <c r="E963" t="s">
+        <v>4054</v>
+      </c>
       <c r="F963" t="s">
         <v>3904</v>
       </c>
@@ -39720,6 +40506,9 @@
       <c r="D964" t="s">
         <v>3907</v>
       </c>
+      <c r="E964" t="s">
+        <v>4055</v>
+      </c>
       <c r="F964" t="s">
         <v>3908</v>
       </c>
@@ -39746,6 +40535,9 @@
       <c r="D965" t="s">
         <v>3911</v>
       </c>
+      <c r="E965" t="s">
+        <v>4054</v>
+      </c>
       <c r="F965" t="s">
         <v>3912</v>
       </c>
@@ -39772,6 +40564,9 @@
       <c r="D966" t="s">
         <v>3915</v>
       </c>
+      <c r="E966" t="s">
+        <v>4053</v>
+      </c>
       <c r="F966" t="s">
         <v>3916</v>
       </c>
@@ -39798,6 +40593,9 @@
       <c r="D967" t="s">
         <v>3918</v>
       </c>
+      <c r="E967" t="s">
+        <v>4054</v>
+      </c>
       <c r="F967" t="s">
         <v>3919</v>
       </c>
@@ -39824,6 +40622,9 @@
       <c r="D968" t="s">
         <v>3921</v>
       </c>
+      <c r="E968" t="s">
+        <v>4053</v>
+      </c>
       <c r="F968" t="s">
         <v>3922</v>
       </c>
@@ -39850,6 +40651,9 @@
       <c r="D969" t="s">
         <v>3925</v>
       </c>
+      <c r="E969" t="s">
+        <v>4054</v>
+      </c>
       <c r="F969" t="s">
         <v>3926</v>
       </c>
@@ -39876,6 +40680,9 @@
       <c r="D970" t="s">
         <v>3928</v>
       </c>
+      <c r="E970" t="s">
+        <v>4055</v>
+      </c>
       <c r="F970" t="s">
         <v>3929</v>
       </c>
@@ -39902,6 +40709,9 @@
       <c r="D971" t="s">
         <v>3932</v>
       </c>
+      <c r="E971" t="s">
+        <v>4054</v>
+      </c>
       <c r="F971" t="s">
         <v>3933</v>
       </c>
@@ -39928,6 +40738,9 @@
       <c r="D972" t="s">
         <v>3936</v>
       </c>
+      <c r="E972" t="s">
+        <v>4053</v>
+      </c>
       <c r="F972" t="s">
         <v>3937</v>
       </c>
@@ -39954,6 +40767,9 @@
       <c r="D973" t="s">
         <v>3940</v>
       </c>
+      <c r="E973" t="s">
+        <v>4056</v>
+      </c>
       <c r="F973" t="s">
         <v>3941</v>
       </c>
@@ -39980,6 +40796,9 @@
       <c r="D974" t="s">
         <v>3944</v>
       </c>
+      <c r="E974" t="s">
+        <v>4054</v>
+      </c>
       <c r="F974" t="s">
         <v>3945</v>
       </c>
@@ -40006,6 +40825,9 @@
       <c r="D975" t="s">
         <v>3948</v>
       </c>
+      <c r="E975" t="s">
+        <v>4054</v>
+      </c>
       <c r="F975" t="s">
         <v>3949</v>
       </c>
@@ -40032,6 +40854,9 @@
       <c r="D976" t="s">
         <v>3952</v>
       </c>
+      <c r="E976" t="s">
+        <v>4055</v>
+      </c>
       <c r="F976" t="s">
         <v>3953</v>
       </c>
@@ -40058,6 +40883,9 @@
       <c r="D977" t="s">
         <v>3956</v>
       </c>
+      <c r="E977" t="s">
+        <v>4053</v>
+      </c>
       <c r="F977" t="s">
         <v>3957</v>
       </c>
@@ -40084,6 +40912,9 @@
       <c r="D978" t="s">
         <v>3960</v>
       </c>
+      <c r="E978" t="s">
+        <v>4055</v>
+      </c>
       <c r="F978" t="s">
         <v>3961</v>
       </c>
@@ -40110,6 +40941,9 @@
       <c r="D979" t="s">
         <v>3964</v>
       </c>
+      <c r="E979" t="s">
+        <v>4053</v>
+      </c>
       <c r="F979" t="s">
         <v>3965</v>
       </c>
@@ -40136,6 +40970,9 @@
       <c r="D980" t="s">
         <v>3967</v>
       </c>
+      <c r="E980" t="s">
+        <v>4054</v>
+      </c>
       <c r="F980" t="s">
         <v>3968</v>
       </c>
@@ -40162,6 +40999,9 @@
       <c r="D981" t="s">
         <v>3971</v>
       </c>
+      <c r="E981" t="s">
+        <v>4053</v>
+      </c>
       <c r="F981" t="s">
         <v>3972</v>
       </c>
@@ -40188,6 +41028,9 @@
       <c r="D982" t="s">
         <v>3975</v>
       </c>
+      <c r="E982" t="s">
+        <v>4054</v>
+      </c>
       <c r="F982" t="s">
         <v>3976</v>
       </c>
@@ -40214,6 +41057,9 @@
       <c r="D983" t="s">
         <v>3979</v>
       </c>
+      <c r="E983" t="s">
+        <v>4054</v>
+      </c>
       <c r="F983" t="s">
         <v>3980</v>
       </c>
@@ -40240,6 +41086,9 @@
       <c r="D984" t="s">
         <v>3983</v>
       </c>
+      <c r="E984" t="s">
+        <v>4054</v>
+      </c>
       <c r="F984" t="s">
         <v>3984</v>
       </c>
@@ -40266,6 +41115,9 @@
       <c r="D985" t="s">
         <v>3987</v>
       </c>
+      <c r="E985" t="s">
+        <v>4054</v>
+      </c>
       <c r="F985" t="s">
         <v>3988</v>
       </c>
@@ -40292,6 +41144,9 @@
       <c r="D986" t="s">
         <v>3991</v>
       </c>
+      <c r="E986" t="s">
+        <v>4054</v>
+      </c>
       <c r="F986" t="s">
         <v>3992</v>
       </c>
@@ -40318,6 +41173,9 @@
       <c r="D987" t="s">
         <v>3995</v>
       </c>
+      <c r="E987" t="s">
+        <v>4054</v>
+      </c>
       <c r="F987" t="s">
         <v>3996</v>
       </c>
@@ -40344,6 +41202,9 @@
       <c r="D988" t="s">
         <v>3999</v>
       </c>
+      <c r="E988" t="s">
+        <v>4054</v>
+      </c>
       <c r="F988" t="s">
         <v>4000</v>
       </c>
@@ -40370,6 +41231,9 @@
       <c r="D989" t="s">
         <v>4003</v>
       </c>
+      <c r="E989" t="s">
+        <v>4054</v>
+      </c>
       <c r="F989" t="s">
         <v>4004</v>
       </c>
@@ -40396,6 +41260,9 @@
       <c r="D990" t="s">
         <v>4007</v>
       </c>
+      <c r="E990" t="s">
+        <v>4053</v>
+      </c>
       <c r="F990" t="s">
         <v>4008</v>
       </c>
@@ -40422,6 +41289,9 @@
       <c r="D991" t="s">
         <v>4011</v>
       </c>
+      <c r="E991" t="s">
+        <v>4053</v>
+      </c>
       <c r="F991" t="s">
         <v>4012</v>
       </c>
@@ -40448,6 +41318,9 @@
       <c r="D992" t="s">
         <v>4015</v>
       </c>
+      <c r="E992" t="s">
+        <v>4055</v>
+      </c>
       <c r="F992" t="s">
         <v>4016</v>
       </c>
@@ -40474,6 +41347,9 @@
       <c r="D993" t="s">
         <v>4018</v>
       </c>
+      <c r="E993" t="s">
+        <v>4054</v>
+      </c>
       <c r="F993" t="s">
         <v>4019</v>
       </c>
@@ -40500,6 +41376,9 @@
       <c r="D994" t="s">
         <v>4022</v>
       </c>
+      <c r="E994" t="s">
+        <v>4055</v>
+      </c>
       <c r="F994" t="s">
         <v>4023</v>
       </c>
@@ -40526,6 +41405,9 @@
       <c r="D995" t="s">
         <v>4026</v>
       </c>
+      <c r="E995" t="s">
+        <v>4054</v>
+      </c>
       <c r="F995" t="s">
         <v>4027</v>
       </c>
@@ -40552,6 +41434,9 @@
       <c r="D996" t="s">
         <v>4030</v>
       </c>
+      <c r="E996" t="s">
+        <v>4053</v>
+      </c>
       <c r="F996" t="s">
         <v>4031</v>
       </c>
@@ -40578,6 +41463,9 @@
       <c r="D997" t="s">
         <v>4034</v>
       </c>
+      <c r="E997" t="s">
+        <v>4053</v>
+      </c>
       <c r="F997" t="s">
         <v>4035</v>
       </c>
@@ -40604,6 +41492,9 @@
       <c r="D998" t="s">
         <v>4038</v>
       </c>
+      <c r="E998" t="s">
+        <v>4053</v>
+      </c>
       <c r="F998" t="s">
         <v>4039</v>
       </c>
@@ -40630,6 +41521,9 @@
       <c r="D999" t="s">
         <v>4042</v>
       </c>
+      <c r="E999" t="s">
+        <v>4053</v>
+      </c>
       <c r="F999" t="s">
         <v>4043</v>
       </c>
@@ -40656,6 +41550,9 @@
       <c r="D1000" t="s">
         <v>4046</v>
       </c>
+      <c r="E1000" t="s">
+        <v>4053</v>
+      </c>
       <c r="F1000" t="s">
         <v>4047</v>
       </c>
@@ -40681,6 +41578,9 @@
       </c>
       <c r="D1001" t="s">
         <v>4050</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>4053</v>
       </c>
       <c r="F1001" t="s">
         <v>4051</v>

</xml_diff>

<commit_message>
format excel sheets and execute annotation notebooks
</commit_message>
<xml_diff>
--- a/Datasets/annotated_dataset/tweets_session_1_1.xlsx
+++ b/Datasets/annotated_dataset/tweets_session_1_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils_hellwig/Desktop/Studium/Masterstudium WS 2022:23/DH Projekt/Twitter_German_Federal_Election_Perception_2021/Datasets/annotated_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4191AB88-FDAE-DC45-9C0F-26F8EDF2EE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DAF3F7-377F-EA4F-B9DE-FC049A2783A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33640" yWindow="500" windowWidth="26520" windowHeight="31640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12556,17 +12556,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A977" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="E997" sqref="E997"/>
+    <sheetView tabSelected="1" topLeftCell="A959" workbookViewId="0">
+      <selection activeCell="E1007" sqref="E1007"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="48.1640625" customWidth="1"/>
     <col min="6" max="6" width="255.6640625" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -12600,7 +12598,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1.4605892657594801E+18</v>
+        <v>1.4605892657594821E+18</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -41597,7 +41595,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001" xr:uid="{61E161B6-B0CE-AF44-992B-727AA0A0560E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1001" xr:uid="{C0B830DE-4D8B-7A44-8A85-C7E251336F40}">
       <formula1>"POSITIVE,NEGATIVE,NEUTRAL,MIXED"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>